<commit_message>
Updates to text of paper
</commit_message>
<xml_diff>
--- a/Code/URE_NNP_positions_NationalAccounts.xlsx
+++ b/Code/URE_NNP_positions_NationalAccounts.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5604ff08deb8de49/Documents/Research/Denmark/IncomeUncertaintyGit/Code/Rcode/Tables/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\edmun\OneDrive\Documents\Research\Denmark\IncomeUncertaintyGit\Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{1F79CEA3-DF36-4705-9498-8CE1AEEDA8F3}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{C2AFC6DA-D60E-4EDA-8C2A-E463C6F14DDB}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="390" yWindow="528" windowWidth="19818" windowHeight="7110" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -893,7 +893,7 @@
   <dimension ref="A1:AF789"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="N2" workbookViewId="0">
-      <selection activeCell="AD18" sqref="AD18"/>
+      <selection activeCell="AC7" sqref="AC7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1224,18 +1224,18 @@
         <v>122</v>
       </c>
       <c r="W6">
-        <v>2.17</v>
+        <v>4.03</v>
       </c>
       <c r="X6">
         <f>U6/W6</f>
-        <v>706.27211966286757</v>
+        <v>380.3003721261594</v>
       </c>
       <c r="Y6">
         <v>0.1</v>
       </c>
       <c r="Z6" s="12">
         <f>X6*Y6/TotalC</f>
-        <v>7.4074829505478376E-2</v>
+        <v>3.988644665679604E-2</v>
       </c>
     </row>
     <row r="7" spans="1:32" x14ac:dyDescent="0.55000000000000004">
@@ -1311,7 +1311,7 @@
       </c>
       <c r="AC7" s="13">
         <f>Z9+Z13</f>
-        <v>-0.24136243661343293</v>
+        <v>-0.39675109072059639</v>
       </c>
     </row>
     <row r="8" spans="1:32" x14ac:dyDescent="0.55000000000000004">
@@ -1425,11 +1425,11 @@
       </c>
       <c r="X9" s="8">
         <f>SUM(X4:X8)</f>
-        <v>708.49226722014134</v>
+        <v>382.52051968343329</v>
       </c>
       <c r="Z9" s="13">
         <f>SUM(Z4:Z8)</f>
-        <v>8.2095932914994299E-2</v>
+        <v>4.7907550066311963E-2</v>
       </c>
       <c r="AB9" t="s">
         <v>136</v>
@@ -1486,14 +1486,14 @@
       </c>
       <c r="X10" s="7">
         <f>AA20-AB20-AC20</f>
-        <v>-626.32049807599992</v>
+        <v>-337.838740664</v>
       </c>
       <c r="Y10" t="s">
         <v>126</v>
       </c>
       <c r="Z10" s="12">
         <f>Z27*Z30/TotalC</f>
-        <v>-0.28412783347694898</v>
+        <v>-0.42344423989152452</v>
       </c>
       <c r="AB10" t="s">
         <v>137</v>
@@ -1541,15 +1541,16 @@
       <c r="W11" t="s">
         <v>112</v>
       </c>
-      <c r="X11">
-        <v>-10</v>
+      <c r="X11" s="7">
+        <f>AB20</f>
+        <v>-5.6002394363922612</v>
       </c>
       <c r="Y11">
         <v>0.2</v>
       </c>
       <c r="Z11" s="12">
         <f>X11*Y11/TotalC</f>
-        <v>-2.0976285894121743E-3</v>
+        <v>-1.174722234932993E-3</v>
       </c>
       <c r="AB11" t="s">
         <v>138</v>
@@ -1616,19 +1617,20 @@
       <c r="W12" t="s">
         <v>113</v>
       </c>
-      <c r="X12">
-        <v>-71</v>
+      <c r="X12" s="7">
+        <f>AC20</f>
+        <v>-38.213969358735085</v>
       </c>
       <c r="Y12">
         <v>0.5</v>
       </c>
       <c r="Z12" s="12">
         <f>X12*Y12/TotalC</f>
-        <v>-3.7232907462066096E-2</v>
+        <v>-2.003967866045088E-2</v>
       </c>
       <c r="AD12">
         <f>AC7/AC9</f>
-        <v>4.0227072768905492</v>
+        <v>6.6125181786766065</v>
       </c>
     </row>
     <row r="13" spans="1:32" x14ac:dyDescent="0.55000000000000004">
@@ -1669,7 +1671,7 @@
       </c>
       <c r="Z13" s="13">
         <f>SUM(Z10:Z12)</f>
-        <v>-0.32345836952842721</v>
+        <v>-0.44465864078690837</v>
       </c>
     </row>
     <row r="14" spans="1:32" x14ac:dyDescent="0.55000000000000004">
@@ -1710,7 +1712,7 @@
       </c>
       <c r="Y14">
         <f>Z10*TotalC/X10</f>
-        <v>0.43253231180149038</v>
+        <v>1.1950557948008886</v>
       </c>
       <c r="Z14" s="12"/>
     </row>
@@ -1790,6 +1792,15 @@
       <c r="W16" t="s">
         <v>110</v>
       </c>
+      <c r="AB16">
+        <v>-9514</v>
+      </c>
+      <c r="AC16">
+        <v>-132681</v>
+      </c>
+      <c r="AD16">
+        <v>-489979.33758025552</v>
+      </c>
     </row>
     <row r="17" spans="4:30" x14ac:dyDescent="0.55000000000000004">
       <c r="E17" s="3" t="s">
@@ -1913,18 +1924,16 @@
       <c r="Z18" t="s">
         <v>115</v>
       </c>
-      <c r="AA18">
-        <v>-243690</v>
-      </c>
       <c r="AB18">
-        <v>-9514</v>
+        <f>AB16*AD18/AD16</f>
+        <v>-5131.8738386353662</v>
       </c>
       <c r="AC18">
-        <v>-132681</v>
+        <f>AC16*AD18/AD16</f>
+        <v>-71568.441537101011</v>
       </c>
       <c r="AD18">
-        <f>AD20*1000000000/AD19</f>
-        <v>-489979.33758025552</v>
+        <v>-264296</v>
       </c>
     </row>
     <row r="19" spans="4:30" x14ac:dyDescent="0.55000000000000004">
@@ -2054,20 +2063,20 @@
         <v>117</v>
       </c>
       <c r="AA20" s="10">
-        <f>AA18*AA19/1000000000</f>
-        <v>-707.54782275000002</v>
+        <f>SUM(AB20:AD20)</f>
+        <v>-381.65294945912734</v>
       </c>
       <c r="AB20" s="10">
         <f>AB18*AB19/1000000000</f>
-        <v>-10.382304724000001</v>
+        <v>-5.6002394363922612</v>
       </c>
       <c r="AC20" s="10">
         <f>AC18*AC19/1000000000</f>
-        <v>-70.845019949999994</v>
-      </c>
-      <c r="AD20" s="8">
-        <f>AA20-AB20-AC20</f>
-        <v>-626.32049807599992</v>
+        <v>-38.213969358735085</v>
+      </c>
+      <c r="AD20" s="10">
+        <f>AD18*AD19/1000000000</f>
+        <v>-337.838740664</v>
       </c>
     </row>
     <row r="21" spans="4:30" x14ac:dyDescent="0.55000000000000004">
@@ -2367,15 +2376,15 @@
         <v>131</v>
       </c>
       <c r="Z27" s="11">
-        <v>-0.54076639999999998</v>
+        <v>-0.80592039999999998</v>
       </c>
       <c r="AB27">
         <f>Z27*Z30</f>
-        <v>-270.90385296147315</v>
+        <v>-403.73614473874784</v>
       </c>
       <c r="AC27">
         <f>AB27*AB26/TotalC</f>
-        <v>-0.3693661835200337</v>
+        <v>-0.55047751185898197</v>
       </c>
     </row>
     <row r="28" spans="4:30" x14ac:dyDescent="0.55000000000000004">
@@ -2602,8 +2611,11 @@
         <f t="shared" si="0"/>
         <v>4845.5089331573936</v>
       </c>
-    </row>
-    <row r="33" spans="5:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="AB32" s="11">
+        <v>264296</v>
+      </c>
+    </row>
+    <row r="33" spans="5:28" x14ac:dyDescent="0.55000000000000004">
       <c r="E33" s="3" t="s">
         <v>14</v>
       </c>
@@ -2639,8 +2651,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="5:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="AB33">
+        <f>AB32*(W19-X19-Y19)/1000000000</f>
+        <v>338.64775071999998</v>
+      </c>
+    </row>
+    <row r="34" spans="5:28" x14ac:dyDescent="0.55000000000000004">
       <c r="E34" s="3" t="s">
         <v>15</v>
       </c>
@@ -2677,7 +2693,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="5:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="5:28" x14ac:dyDescent="0.55000000000000004">
       <c r="E35" s="3" t="s">
         <v>16</v>
       </c>
@@ -2714,7 +2730,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="5:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="5:28" x14ac:dyDescent="0.55000000000000004">
       <c r="E36" s="3" t="s">
         <v>17</v>
       </c>
@@ -2751,7 +2767,7 @@
         <v>283.25244831301319</v>
       </c>
     </row>
-    <row r="37" spans="5:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="5:28" x14ac:dyDescent="0.55000000000000004">
       <c r="E37" s="3" t="s">
         <v>18</v>
       </c>
@@ -2788,7 +2804,7 @@
         <v>13.386830853674757</v>
       </c>
     </row>
-    <row r="38" spans="5:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="5:28" x14ac:dyDescent="0.55000000000000004">
       <c r="E38" s="3" t="s">
         <v>19</v>
       </c>
@@ -2825,7 +2841,7 @@
         <v>195.40766107375495</v>
       </c>
     </row>
-    <row r="39" spans="5:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="5:28" x14ac:dyDescent="0.55000000000000004">
       <c r="E39" s="3" t="s">
         <v>20</v>
       </c>
@@ -2862,7 +2878,7 @@
         <v>74.749778223807866</v>
       </c>
     </row>
-    <row r="40" spans="5:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="5:28" x14ac:dyDescent="0.55000000000000004">
       <c r="E40" s="3" t="s">
         <v>21</v>
       </c>
@@ -2899,7 +2915,7 @@
         <v>129.21356840539235</v>
       </c>
     </row>
-    <row r="41" spans="5:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="5:28" x14ac:dyDescent="0.55000000000000004">
       <c r="E41" s="3" t="s">
         <v>22</v>
       </c>
@@ -2936,7 +2952,7 @@
         <v>7.3697718741785962</v>
       </c>
     </row>
-    <row r="42" spans="5:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="5:28" x14ac:dyDescent="0.55000000000000004">
       <c r="E42" s="3" t="s">
         <v>23</v>
       </c>
@@ -2973,7 +2989,7 @@
         <v>121.84379653121375</v>
       </c>
     </row>
-    <row r="43" spans="5:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="5:28" x14ac:dyDescent="0.55000000000000004">
       <c r="E43" s="3" t="s">
         <v>24</v>
       </c>
@@ -3010,7 +3026,7 @@
         <v>815.17884617900677</v>
       </c>
     </row>
-    <row r="44" spans="5:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="44" spans="5:28" x14ac:dyDescent="0.55000000000000004">
       <c r="E44" s="3" t="s">
         <v>25</v>
       </c>
@@ -3047,7 +3063,7 @@
         <v>689.85757009531278</v>
       </c>
     </row>
-    <row r="45" spans="5:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="5:28" x14ac:dyDescent="0.55000000000000004">
       <c r="E45" s="3" t="s">
         <v>26</v>
       </c>
@@ -3084,7 +3100,7 @@
         <v>125.47024077906121</v>
       </c>
     </row>
-    <row r="46" spans="5:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" spans="5:28" x14ac:dyDescent="0.55000000000000004">
       <c r="E46" s="3" t="s">
         <v>27</v>
       </c>
@@ -3121,7 +3137,7 @@
         <v>2599.4667089249865</v>
       </c>
     </row>
-    <row r="47" spans="5:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="47" spans="5:28" x14ac:dyDescent="0.55000000000000004">
       <c r="E47" s="3" t="s">
         <v>28</v>
       </c>
@@ -3158,7 +3174,7 @@
         <v>90.15783609834854</v>
       </c>
     </row>
-    <row r="48" spans="5:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="48" spans="5:28" x14ac:dyDescent="0.55000000000000004">
       <c r="E48" s="3" t="s">
         <v>29</v>
       </c>

</xml_diff>